<commit_message>
FIX:se arreglo algunos nombres de los professores y se agrego informacion de los indigenas
</commit_message>
<xml_diff>
--- a/downloads/INSCRITOS_TODOS.xlsx
+++ b/downloads/INSCRITOS_TODOS.xlsx
@@ -10,7 +10,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$C$1:$H$64</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$C$1:$H$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$C$1:$H$317</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
@@ -1786,7 +1786,7 @@
     <t>191</t>
   </si>
   <si>
-    <t xml:space="preserve">ARIVELTON RIBERO FREITAS</t>
+    <t xml:space="preserve">ARIVELTON RIBEIRO FREITAS</t>
   </si>
   <si>
     <t xml:space="preserve">BRUNO AMORIM DA SILVA</t>
@@ -1996,7 +1996,7 @@
     <t xml:space="preserve">MARIA NILMA TAVARES DE OLIVEIRA</t>
   </si>
   <si>
-    <t xml:space="preserve">MARIA RAIANE EMANUELY LIMAPENEDO</t>
+    <t xml:space="preserve">MARIA RAIANE EMANUELY LIMA PENEDO</t>
   </si>
   <si>
     <t>162</t>
@@ -2044,7 +2044,7 @@
     <t>022</t>
   </si>
   <si>
-    <t xml:space="preserve">RAIMUNDO MACIEL OVARTE</t>
+    <t xml:space="preserve">RAIMUNDO MACIEL DUARTE</t>
   </si>
   <si>
     <t>154</t>
@@ -2142,7 +2142,6 @@
     <font>
       <b/>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Arial Narrow"/>
     </font>
     <font>
@@ -2152,7 +2151,6 @@
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Arial Narrow"/>
     </font>
     <font>
@@ -2221,7 +2219,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" vertical="center" wrapText="1"/>
@@ -2268,9 +2266,6 @@
     </xf>
     <xf fontId="5" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4513,10 +4508,10 @@
       <c r="D65" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E65" s="19" t="s">
+      <c r="E65" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F65" s="20" t="s">
+      <c r="F65" s="19" t="s">
         <v>178</v>
       </c>
       <c r="G65" s="17" t="s">
@@ -4539,10 +4534,10 @@
       <c r="D66" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E66" s="19" t="s">
+      <c r="E66" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F66" s="20" t="s">
+      <c r="F66" s="19" t="s">
         <v>181</v>
       </c>
       <c r="G66" s="17" t="s">
@@ -4565,10 +4560,10 @@
       <c r="D67" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E67" s="19" t="s">
+      <c r="E67" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="F67" s="20" t="s">
+      <c r="F67" s="19" t="s">
         <v>184</v>
       </c>
       <c r="G67" s="17" t="s">
@@ -4591,10 +4586,10 @@
       <c r="D68" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E68" s="19" t="s">
+      <c r="E68" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="F68" s="20" t="s">
+      <c r="F68" s="19" t="s">
         <v>187</v>
       </c>
       <c r="G68" s="17" t="s">
@@ -4617,10 +4612,10 @@
       <c r="D69" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E69" s="19" t="s">
+      <c r="E69" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="F69" s="20" t="s">
+      <c r="F69" s="19" t="s">
         <v>181</v>
       </c>
       <c r="G69" s="17" t="s">
@@ -4643,10 +4638,10 @@
       <c r="D70" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E70" s="19" t="s">
+      <c r="E70" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F70" s="20" t="s">
+      <c r="F70" s="19" t="s">
         <v>80</v>
       </c>
       <c r="G70" s="17" t="s">
@@ -4669,10 +4664,10 @@
       <c r="D71" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E71" s="19" t="s">
+      <c r="E71" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F71" s="20" t="s">
+      <c r="F71" s="19" t="s">
         <v>192</v>
       </c>
       <c r="G71" s="17" t="s">
@@ -4695,10 +4690,10 @@
       <c r="D72" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E72" s="19" t="s">
+      <c r="E72" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F72" s="20" t="s">
+      <c r="F72" s="19" t="s">
         <v>194</v>
       </c>
       <c r="G72" s="17" t="s">
@@ -4721,10 +4716,10 @@
       <c r="D73" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E73" s="19" t="s">
+      <c r="E73" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="F73" s="20" t="s">
+      <c r="F73" s="19" t="s">
         <v>181</v>
       </c>
       <c r="G73" s="17" t="s">
@@ -4747,10 +4742,10 @@
       <c r="D74" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E74" s="19" t="s">
+      <c r="E74" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="F74" s="20" t="s">
+      <c r="F74" s="19" t="s">
         <v>200</v>
       </c>
       <c r="G74" s="17" t="s">
@@ -4773,10 +4768,10 @@
       <c r="D75" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E75" s="19" t="s">
+      <c r="E75" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="F75" s="20" t="s">
+      <c r="F75" s="19" t="s">
         <v>178</v>
       </c>
       <c r="G75" s="17" t="s">
@@ -4799,10 +4794,10 @@
       <c r="D76" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E76" s="19" t="s">
+      <c r="E76" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="F76" s="20" t="s">
+      <c r="F76" s="19" t="s">
         <v>181</v>
       </c>
       <c r="G76" s="17" t="s">
@@ -4825,10 +4820,10 @@
       <c r="D77" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E77" s="19" t="s">
+      <c r="E77" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="F77" s="20" t="s">
+      <c r="F77" s="19" t="s">
         <v>207</v>
       </c>
       <c r="G77" s="17" t="s">
@@ -4851,10 +4846,10 @@
       <c r="D78" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E78" s="19" t="s">
+      <c r="E78" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="F78" s="20" t="s">
+      <c r="F78" s="19" t="s">
         <v>212</v>
       </c>
       <c r="G78" s="17" t="s">
@@ -4877,10 +4872,10 @@
       <c r="D79" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E79" s="19" t="s">
+      <c r="E79" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="F79" s="20" t="s">
+      <c r="F79" s="19" t="s">
         <v>217</v>
       </c>
       <c r="G79" s="17" t="s">
@@ -4903,10 +4898,10 @@
       <c r="D80" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E80" s="19" t="s">
+      <c r="E80" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="F80" s="20" t="s">
+      <c r="F80" s="19" t="s">
         <v>217</v>
       </c>
       <c r="G80" s="17" t="s">
@@ -4929,10 +4924,10 @@
       <c r="D81" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E81" s="19" t="s">
+      <c r="E81" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="F81" s="20" t="s">
+      <c r="F81" s="19" t="s">
         <v>224</v>
       </c>
       <c r="G81" s="17" t="s">
@@ -4955,10 +4950,10 @@
       <c r="D82" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E82" s="19" t="s">
+      <c r="E82" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="F82" s="20" t="s">
+      <c r="F82" s="19" t="s">
         <v>178</v>
       </c>
       <c r="G82" s="17" t="s">
@@ -4981,10 +4976,10 @@
       <c r="D83" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E83" s="19" t="s">
+      <c r="E83" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="F83" s="20" t="s">
+      <c r="F83" s="19" t="s">
         <v>229</v>
       </c>
       <c r="G83" s="17" t="s">
@@ -5007,10 +5002,10 @@
       <c r="D84" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E84" s="19" t="s">
+      <c r="E84" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="F84" s="20" t="s">
+      <c r="F84" s="19" t="s">
         <v>224</v>
       </c>
       <c r="G84" s="17" t="s">
@@ -5033,10 +5028,10 @@
       <c r="D85" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E85" s="19" t="s">
+      <c r="E85" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="F85" s="20" t="s">
+      <c r="F85" s="19" t="s">
         <v>217</v>
       </c>
       <c r="G85" s="17" t="s">
@@ -5059,10 +5054,10 @@
       <c r="D86" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E86" s="19" t="s">
+      <c r="E86" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="F86" s="20" t="s">
+      <c r="F86" s="19" t="s">
         <v>207</v>
       </c>
       <c r="G86" s="17" t="s">
@@ -5085,10 +5080,10 @@
       <c r="D87" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E87" s="19" t="s">
+      <c r="E87" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="F87" s="20" t="s">
+      <c r="F87" s="19" t="s">
         <v>238</v>
       </c>
       <c r="G87" s="17" t="s">
@@ -5111,10 +5106,10 @@
       <c r="D88" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E88" s="19" t="s">
+      <c r="E88" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="F88" s="20" t="s">
+      <c r="F88" s="19" t="s">
         <v>200</v>
       </c>
       <c r="G88" s="17" t="s">
@@ -5137,10 +5132,10 @@
       <c r="D89" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E89" s="19" t="s">
+      <c r="E89" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="F89" s="20" t="s">
+      <c r="F89" s="19" t="s">
         <v>200</v>
       </c>
       <c r="G89" s="17" t="s">
@@ -5163,10 +5158,10 @@
       <c r="D90" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E90" s="19" t="s">
+      <c r="E90" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="F90" s="20" t="s">
+      <c r="F90" s="19" t="s">
         <v>244</v>
       </c>
       <c r="G90" s="17" t="s">
@@ -5189,10 +5184,10 @@
       <c r="D91" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E91" s="19" t="s">
+      <c r="E91" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="F91" s="20" t="s">
+      <c r="F91" s="19" t="s">
         <v>238</v>
       </c>
       <c r="G91" s="17" t="s">
@@ -5215,10 +5210,10 @@
       <c r="D92" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E92" s="19" t="s">
+      <c r="E92" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="F92" s="20" t="s">
+      <c r="F92" s="19" t="s">
         <v>250</v>
       </c>
       <c r="G92" s="17" t="s">
@@ -5241,10 +5236,10 @@
       <c r="D93" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E93" s="19" t="s">
+      <c r="E93" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="F93" s="20" t="s">
+      <c r="F93" s="19" t="s">
         <v>12</v>
       </c>
       <c r="G93" s="17" t="s">
@@ -5267,10 +5262,10 @@
       <c r="D94" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E94" s="19" t="s">
+      <c r="E94" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="F94" s="20" t="s">
+      <c r="F94" s="19" t="s">
         <v>238</v>
       </c>
       <c r="G94" s="17" t="s">
@@ -5293,10 +5288,10 @@
       <c r="D95" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E95" s="19" t="s">
+      <c r="E95" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="F95" s="20" t="s">
+      <c r="F95" s="19" t="s">
         <v>257</v>
       </c>
       <c r="G95" s="17" t="s">
@@ -5319,10 +5314,10 @@
       <c r="D96" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E96" s="19" t="s">
+      <c r="E96" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="F96" s="20" t="s">
+      <c r="F96" s="19" t="s">
         <v>80</v>
       </c>
       <c r="G96" s="17" t="s">
@@ -5345,10 +5340,10 @@
       <c r="D97" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E97" s="19" t="s">
+      <c r="E97" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="F97" s="20" t="s">
+      <c r="F97" s="19" t="s">
         <v>187</v>
       </c>
       <c r="G97" s="17" t="s">
@@ -5371,10 +5366,10 @@
       <c r="D98" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E98" s="19" t="s">
+      <c r="E98" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="F98" s="20" t="s">
+      <c r="F98" s="19" t="s">
         <v>181</v>
       </c>
       <c r="G98" s="17" t="s">
@@ -5397,10 +5392,10 @@
       <c r="D99" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E99" s="19" t="s">
+      <c r="E99" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="F99" s="20" t="s">
+      <c r="F99" s="19" t="s">
         <v>181</v>
       </c>
       <c r="G99" s="17" t="s">
@@ -5423,10 +5418,10 @@
       <c r="D100" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E100" s="19" t="s">
+      <c r="E100" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="F100" s="20" t="s">
+      <c r="F100" s="19" t="s">
         <v>192</v>
       </c>
       <c r="G100" s="17" t="s">
@@ -5449,10 +5444,10 @@
       <c r="D101" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E101" s="19" t="s">
+      <c r="E101" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="F101" s="20" t="s">
+      <c r="F101" s="19" t="s">
         <v>192</v>
       </c>
       <c r="G101" s="17" t="s">
@@ -5475,10 +5470,10 @@
       <c r="D102" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E102" s="19" t="s">
+      <c r="E102" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F102" s="20" t="s">
+      <c r="F102" s="19" t="s">
         <v>207</v>
       </c>
       <c r="G102" s="17" t="s">
@@ -5501,10 +5496,10 @@
       <c r="D103" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E103" s="19" t="s">
+      <c r="E103" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="F103" s="20" t="s">
+      <c r="F103" s="19" t="s">
         <v>270</v>
       </c>
       <c r="G103" s="17" t="s">
@@ -5527,10 +5522,10 @@
       <c r="D104" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E104" s="19" t="s">
+      <c r="E104" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="F104" s="20" t="s">
+      <c r="F104" s="19" t="s">
         <v>224</v>
       </c>
       <c r="G104" s="17" t="s">
@@ -5553,10 +5548,10 @@
       <c r="D105" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E105" s="19" t="s">
+      <c r="E105" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="F105" s="20" t="s">
+      <c r="F105" s="19" t="s">
         <v>276</v>
       </c>
       <c r="G105" s="17" t="s">
@@ -5579,10 +5574,10 @@
       <c r="D106" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E106" s="19" t="s">
+      <c r="E106" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="F106" s="20" t="s">
+      <c r="F106" s="19" t="s">
         <v>279</v>
       </c>
       <c r="G106" s="17" t="s">
@@ -5605,10 +5600,10 @@
       <c r="D107" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E107" s="19" t="s">
+      <c r="E107" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="F107" s="20" t="s">
+      <c r="F107" s="19" t="s">
         <v>178</v>
       </c>
       <c r="G107" s="17" t="s">
@@ -5631,10 +5626,10 @@
       <c r="D108" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E108" s="19" t="s">
+      <c r="E108" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F108" s="20" t="s">
+      <c r="F108" s="19" t="s">
         <v>80</v>
       </c>
       <c r="G108" s="17" t="s">
@@ -5657,10 +5652,10 @@
       <c r="D109" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E109" s="19" t="s">
+      <c r="E109" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="F109" s="20" t="s">
+      <c r="F109" s="19" t="s">
         <v>181</v>
       </c>
       <c r="G109" s="17" t="s">
@@ -5683,10 +5678,10 @@
       <c r="D110" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E110" s="19" t="s">
+      <c r="E110" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="F110" s="20" t="s">
+      <c r="F110" s="19" t="s">
         <v>80</v>
       </c>
       <c r="G110" s="17" t="s">
@@ -5709,10 +5704,10 @@
       <c r="D111" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E111" s="19" t="s">
+      <c r="E111" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="F111" s="20" t="s">
+      <c r="F111" s="19" t="s">
         <v>217</v>
       </c>
       <c r="G111" s="17" t="s">
@@ -5735,10 +5730,10 @@
       <c r="D112" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E112" s="19" t="s">
+      <c r="E112" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="F112" s="20" t="s">
+      <c r="F112" s="19" t="s">
         <v>200</v>
       </c>
       <c r="G112" s="17" t="s">
@@ -5761,10 +5756,10 @@
       <c r="D113" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E113" s="19" t="s">
+      <c r="E113" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="F113" s="20" t="s">
+      <c r="F113" s="19" t="s">
         <v>293</v>
       </c>
       <c r="G113" s="17" t="s">
@@ -5787,10 +5782,10 @@
       <c r="D114" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E114" s="19" t="s">
+      <c r="E114" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="F114" s="20" t="s">
+      <c r="F114" s="19" t="s">
         <v>184</v>
       </c>
       <c r="G114" s="17" t="s">
@@ -5813,10 +5808,10 @@
       <c r="D115" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E115" s="19" t="s">
+      <c r="E115" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="F115" s="20" t="s">
+      <c r="F115" s="19" t="s">
         <v>181</v>
       </c>
       <c r="G115" s="17" t="s">
@@ -5839,10 +5834,10 @@
       <c r="D116" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E116" s="19" t="s">
+      <c r="E116" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="F116" s="20" t="s">
+      <c r="F116" s="19" t="s">
         <v>187</v>
       </c>
       <c r="G116" s="17" t="s">
@@ -5865,13 +5860,13 @@
       <c r="D117" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E117" s="21" t="s">
+      <c r="E117" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F117" s="22" t="s">
+      <c r="F117" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G117" s="23" t="s">
+      <c r="G117" s="22" t="s">
         <v>25</v>
       </c>
       <c r="H117" s="11" t="s">
@@ -5891,7 +5886,7 @@
       <c r="D118" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E118" s="21" t="s">
+      <c r="E118" s="20" t="s">
         <v>302</v>
       </c>
       <c r="F118" s="13" t="s">
@@ -5917,7 +5912,7 @@
       <c r="D119" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E119" s="21">
+      <c r="E119" s="20">
         <v>224</v>
       </c>
       <c r="F119" s="13" t="s">
@@ -5943,7 +5938,7 @@
       <c r="D120" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E120" s="21">
+      <c r="E120" s="20">
         <v>222</v>
       </c>
       <c r="F120" s="13" t="s">
@@ -5969,7 +5964,7 @@
       <c r="D121" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E121" s="21" t="s">
+      <c r="E121" s="20" t="s">
         <v>309</v>
       </c>
       <c r="F121" s="13" t="s">
@@ -5995,7 +5990,7 @@
       <c r="D122" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E122" s="21" t="s">
+      <c r="E122" s="20" t="s">
         <v>149</v>
       </c>
       <c r="F122" s="13" t="s">
@@ -6021,7 +6016,7 @@
       <c r="D123" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E123" s="21" t="s">
+      <c r="E123" s="20" t="s">
         <v>131</v>
       </c>
       <c r="F123" s="13" t="s">
@@ -6047,7 +6042,7 @@
       <c r="D124" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E124" s="21" t="s">
+      <c r="E124" s="20" t="s">
         <v>313</v>
       </c>
       <c r="F124" s="13" t="s">
@@ -6073,7 +6068,7 @@
       <c r="D125" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E125" s="21" t="s">
+      <c r="E125" s="20" t="s">
         <v>317</v>
       </c>
       <c r="F125" s="13" t="s">
@@ -6099,7 +6094,7 @@
       <c r="D126" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E126" s="21" t="s">
+      <c r="E126" s="20" t="s">
         <v>85</v>
       </c>
       <c r="F126" s="13" t="s">
@@ -6125,7 +6120,7 @@
       <c r="D127" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E127" s="21" t="s">
+      <c r="E127" s="20" t="s">
         <v>321</v>
       </c>
       <c r="F127" s="13" t="s">
@@ -6151,7 +6146,7 @@
       <c r="D128" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E128" s="21" t="s">
+      <c r="E128" s="20" t="s">
         <v>323</v>
       </c>
       <c r="F128" s="13" t="s">
@@ -6177,7 +6172,7 @@
       <c r="D129" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E129" s="21" t="s">
+      <c r="E129" s="20" t="s">
         <v>327</v>
       </c>
       <c r="F129" s="13" t="s">
@@ -6203,7 +6198,7 @@
       <c r="D130" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E130" s="21" t="s">
+      <c r="E130" s="20" t="s">
         <v>331</v>
       </c>
       <c r="F130" s="13" t="s">
@@ -6229,7 +6224,7 @@
       <c r="D131" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E131" s="21" t="s">
+      <c r="E131" s="20" t="s">
         <v>40</v>
       </c>
       <c r="F131" s="13" t="s">
@@ -6255,7 +6250,7 @@
       <c r="D132" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E132" s="21" t="s">
+      <c r="E132" s="20" t="s">
         <v>334</v>
       </c>
       <c r="F132" s="13" t="s">
@@ -6281,7 +6276,7 @@
       <c r="D133" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E133" s="21" t="s">
+      <c r="E133" s="20" t="s">
         <v>338</v>
       </c>
       <c r="F133" s="13" t="s">
@@ -6307,7 +6302,7 @@
       <c r="D134" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E134" s="21" t="s">
+      <c r="E134" s="20" t="s">
         <v>123</v>
       </c>
       <c r="F134" s="13" t="s">
@@ -6333,7 +6328,7 @@
       <c r="D135" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E135" s="21" t="s">
+      <c r="E135" s="20" t="s">
         <v>341</v>
       </c>
       <c r="F135" s="13" t="s">
@@ -6359,7 +6354,7 @@
       <c r="D136" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E136" s="21" t="s">
+      <c r="E136" s="20" t="s">
         <v>344</v>
       </c>
       <c r="F136" s="13" t="s">
@@ -6385,7 +6380,7 @@
       <c r="D137" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E137" s="21" t="s">
+      <c r="E137" s="20" t="s">
         <v>346</v>
       </c>
       <c r="F137" s="13" t="s">
@@ -6411,7 +6406,7 @@
       <c r="D138" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E138" s="21" t="s">
+      <c r="E138" s="20" t="s">
         <v>348</v>
       </c>
       <c r="F138" s="13" t="s">
@@ -6437,7 +6432,7 @@
       <c r="D139" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E139" s="21" t="s">
+      <c r="E139" s="20" t="s">
         <v>350</v>
       </c>
       <c r="F139" s="13" t="s">
@@ -6463,7 +6458,7 @@
       <c r="D140" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E140" s="21" t="s">
+      <c r="E140" s="20" t="s">
         <v>352</v>
       </c>
       <c r="F140" s="13" t="s">
@@ -6489,7 +6484,7 @@
       <c r="D141" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E141" s="21" t="s">
+      <c r="E141" s="20" t="s">
         <v>357</v>
       </c>
       <c r="F141" s="13" t="s">
@@ -6515,7 +6510,7 @@
       <c r="D142" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E142" s="21" t="s">
+      <c r="E142" s="20" t="s">
         <v>359</v>
       </c>
       <c r="F142" s="13" t="s">
@@ -6541,7 +6536,7 @@
       <c r="D143" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E143" s="21" t="s">
+      <c r="E143" s="20" t="s">
         <v>90</v>
       </c>
       <c r="F143" s="13" t="s">
@@ -6567,7 +6562,7 @@
       <c r="D144" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E144" s="21" t="s">
+      <c r="E144" s="20" t="s">
         <v>362</v>
       </c>
       <c r="F144" s="13" t="s">
@@ -6593,7 +6588,7 @@
       <c r="D145" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E145" s="21" t="s">
+      <c r="E145" s="20" t="s">
         <v>364</v>
       </c>
       <c r="F145" s="13" t="s">
@@ -6619,7 +6614,7 @@
       <c r="D146" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E146" s="21" t="s">
+      <c r="E146" s="20" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="13" t="s">
@@ -6645,7 +6640,7 @@
       <c r="D147" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E147" s="21" t="s">
+      <c r="E147" s="20" t="s">
         <v>367</v>
       </c>
       <c r="F147" s="13" t="s">
@@ -6671,7 +6666,7 @@
       <c r="D148" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E148" s="21" t="s">
+      <c r="E148" s="20" t="s">
         <v>371</v>
       </c>
       <c r="F148" s="13" t="s">
@@ -6697,7 +6692,7 @@
       <c r="D149" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E149" s="21" t="s">
+      <c r="E149" s="20" t="s">
         <v>373</v>
       </c>
       <c r="F149" s="13" t="s">
@@ -6723,7 +6718,7 @@
       <c r="D150" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E150" s="21" t="s">
+      <c r="E150" s="20" t="s">
         <v>375</v>
       </c>
       <c r="F150" s="13" t="s">
@@ -6749,7 +6744,7 @@
       <c r="D151" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E151" s="21" t="s">
+      <c r="E151" s="20" t="s">
         <v>379</v>
       </c>
       <c r="F151" s="13" t="s">
@@ -6775,7 +6770,7 @@
       <c r="D152" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E152" s="21" t="s">
+      <c r="E152" s="20" t="s">
         <v>381</v>
       </c>
       <c r="F152" s="13" t="s">
@@ -6801,7 +6796,7 @@
       <c r="D153" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E153" s="21" t="s">
+      <c r="E153" s="20" t="s">
         <v>383</v>
       </c>
       <c r="F153" s="13" t="s">
@@ -6827,7 +6822,7 @@
       <c r="D154" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E154" s="21" t="s">
+      <c r="E154" s="20" t="s">
         <v>385</v>
       </c>
       <c r="F154" s="13" t="s">
@@ -6853,7 +6848,7 @@
       <c r="D155" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E155" s="21" t="s">
+      <c r="E155" s="20" t="s">
         <v>387</v>
       </c>
       <c r="F155" s="13" t="s">
@@ -6879,7 +6874,7 @@
       <c r="D156" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E156" s="21" t="s">
+      <c r="E156" s="20" t="s">
         <v>389</v>
       </c>
       <c r="F156" s="13" t="s">
@@ -6905,7 +6900,7 @@
       <c r="D157" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E157" s="21">
+      <c r="E157" s="20">
         <v>244</v>
       </c>
       <c r="F157" s="13" t="s">
@@ -6931,7 +6926,7 @@
       <c r="D158" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E158" s="21" t="s">
+      <c r="E158" s="20" t="s">
         <v>394</v>
       </c>
       <c r="F158" s="13" t="s">
@@ -6957,7 +6952,7 @@
       <c r="D159" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E159" s="21" t="s">
+      <c r="E159" s="20" t="s">
         <v>67</v>
       </c>
       <c r="F159" s="13" t="s">
@@ -6983,7 +6978,7 @@
       <c r="D160" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E160" s="21" t="s">
+      <c r="E160" s="20" t="s">
         <v>397</v>
       </c>
       <c r="F160" s="13" t="s">
@@ -7009,7 +7004,7 @@
       <c r="D161" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E161" s="21" t="s">
+      <c r="E161" s="20" t="s">
         <v>399</v>
       </c>
       <c r="F161" s="13" t="s">
@@ -7035,7 +7030,7 @@
       <c r="D162" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E162" s="21" t="s">
+      <c r="E162" s="20" t="s">
         <v>401</v>
       </c>
       <c r="F162" s="13" t="s">
@@ -7061,7 +7056,7 @@
       <c r="D163" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E163" s="21" t="s">
+      <c r="E163" s="20" t="s">
         <v>403</v>
       </c>
       <c r="F163" s="13" t="s">
@@ -7087,7 +7082,7 @@
       <c r="D164" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E164" s="21" t="s">
+      <c r="E164" s="20" t="s">
         <v>83</v>
       </c>
       <c r="F164" s="13" t="s">
@@ -7113,7 +7108,7 @@
       <c r="D165" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E165" s="21" t="s">
+      <c r="E165" s="20" t="s">
         <v>406</v>
       </c>
       <c r="F165" s="13" t="s">
@@ -7139,7 +7134,7 @@
       <c r="D166" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E166" s="21" t="s">
+      <c r="E166" s="20" t="s">
         <v>408</v>
       </c>
       <c r="F166" s="13" t="s">
@@ -7165,10 +7160,10 @@
       <c r="D167" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E167" s="19" t="s">
+      <c r="E167" s="12" t="s">
         <v>410</v>
       </c>
-      <c r="F167" s="20" t="s">
+      <c r="F167" s="19" t="s">
         <v>50</v>
       </c>
       <c r="G167" s="17" t="s">
@@ -7191,10 +7186,10 @@
       <c r="D168" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E168" s="19" t="s">
+      <c r="E168" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F168" s="20" t="s">
+      <c r="F168" s="19" t="s">
         <v>412</v>
       </c>
       <c r="G168" s="17" t="s">
@@ -7217,10 +7212,10 @@
       <c r="D169" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E169" s="19" t="s">
+      <c r="E169" s="12" t="s">
         <v>414</v>
       </c>
-      <c r="F169" s="20" t="s">
+      <c r="F169" s="19" t="s">
         <v>412</v>
       </c>
       <c r="G169" s="17" t="s">
@@ -7243,10 +7238,10 @@
       <c r="D170" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E170" s="19" t="s">
+      <c r="E170" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="F170" s="20" t="s">
+      <c r="F170" s="19" t="s">
         <v>24</v>
       </c>
       <c r="G170" s="17" t="s">
@@ -7269,10 +7264,10 @@
       <c r="D171" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E171" s="19" t="s">
+      <c r="E171" s="12" t="s">
         <v>418</v>
       </c>
-      <c r="F171" s="20" t="s">
+      <c r="F171" s="19" t="s">
         <v>419</v>
       </c>
       <c r="G171" s="17" t="s">
@@ -7295,10 +7290,10 @@
       <c r="D172" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E172" s="19" t="s">
+      <c r="E172" s="12" t="s">
         <v>423</v>
       </c>
-      <c r="F172" s="20" t="s">
+      <c r="F172" s="19" t="s">
         <v>59</v>
       </c>
       <c r="G172" s="17" t="s">
@@ -7321,10 +7316,10 @@
       <c r="D173" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E173" s="19" t="s">
+      <c r="E173" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="F173" s="20" t="s">
+      <c r="F173" s="19" t="s">
         <v>24</v>
       </c>
       <c r="G173" s="17" t="s">
@@ -7347,10 +7342,10 @@
       <c r="D174" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E174" s="19" t="s">
+      <c r="E174" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="F174" s="20" t="s">
+      <c r="F174" s="19" t="s">
         <v>24</v>
       </c>
       <c r="G174" s="17" t="s">
@@ -7373,10 +7368,10 @@
       <c r="D175" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E175" s="19" t="s">
+      <c r="E175" s="12" t="s">
         <v>428</v>
       </c>
-      <c r="F175" s="20" t="s">
+      <c r="F175" s="19" t="s">
         <v>59</v>
       </c>
       <c r="G175" s="17" t="s">
@@ -7399,10 +7394,10 @@
       <c r="D176" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E176" s="19" t="s">
+      <c r="E176" s="12" t="s">
         <v>430</v>
       </c>
-      <c r="F176" s="20" t="s">
+      <c r="F176" s="19" t="s">
         <v>59</v>
       </c>
       <c r="G176" s="17" t="s">
@@ -7425,10 +7420,10 @@
       <c r="D177" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E177" s="19" t="s">
+      <c r="E177" s="12" t="s">
         <v>432</v>
       </c>
-      <c r="F177" s="20" t="s">
+      <c r="F177" s="19" t="s">
         <v>433</v>
       </c>
       <c r="G177" s="17" t="s">
@@ -7451,10 +7446,10 @@
       <c r="D178" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E178" s="19" t="s">
+      <c r="E178" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="F178" s="20" t="s">
+      <c r="F178" s="19" t="s">
         <v>412</v>
       </c>
       <c r="G178" s="17" t="s">
@@ -7477,10 +7472,10 @@
       <c r="D179" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E179" s="19" t="s">
+      <c r="E179" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="F179" s="20" t="s">
+      <c r="F179" s="19" t="s">
         <v>276</v>
       </c>
       <c r="G179" s="17" t="s">
@@ -7503,10 +7498,10 @@
       <c r="D180" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E180" s="19" t="s">
+      <c r="E180" s="12" t="s">
         <v>440</v>
       </c>
-      <c r="F180" s="20" t="s">
+      <c r="F180" s="19" t="s">
         <v>441</v>
       </c>
       <c r="G180" s="17" t="s">
@@ -7529,10 +7524,10 @@
       <c r="D181" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E181" s="19" t="s">
+      <c r="E181" s="12" t="s">
         <v>443</v>
       </c>
-      <c r="F181" s="20" t="s">
+      <c r="F181" s="19" t="s">
         <v>24</v>
       </c>
       <c r="G181" s="17" t="s">
@@ -7555,10 +7550,10 @@
       <c r="D182" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E182" s="19" t="s">
+      <c r="E182" s="12" t="s">
         <v>445</v>
       </c>
-      <c r="F182" s="20" t="s">
+      <c r="F182" s="19" t="s">
         <v>446</v>
       </c>
       <c r="G182" s="17" t="s">
@@ -7581,10 +7576,10 @@
       <c r="D183" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E183" s="19" t="s">
+      <c r="E183" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="F183" s="20" t="s">
+      <c r="F183" s="19" t="s">
         <v>441</v>
       </c>
       <c r="G183" s="17" t="s">
@@ -7607,10 +7602,10 @@
       <c r="D184" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E184" s="19" t="s">
+      <c r="E184" s="12" t="s">
         <v>451</v>
       </c>
-      <c r="F184" s="20" t="s">
+      <c r="F184" s="19" t="s">
         <v>276</v>
       </c>
       <c r="G184" s="17" t="s">
@@ -7633,10 +7628,10 @@
       <c r="D185" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E185" s="19" t="s">
+      <c r="E185" s="12" t="s">
         <v>453</v>
       </c>
-      <c r="F185" s="20" t="s">
+      <c r="F185" s="19" t="s">
         <v>50</v>
       </c>
       <c r="G185" s="17" t="s">
@@ -7659,10 +7654,10 @@
       <c r="D186" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E186" s="19" t="s">
+      <c r="E186" s="12" t="s">
         <v>455</v>
       </c>
-      <c r="F186" s="20" t="s">
+      <c r="F186" s="19" t="s">
         <v>24</v>
       </c>
       <c r="G186" s="17" t="s">
@@ -7685,10 +7680,10 @@
       <c r="D187" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E187" s="19" t="s">
+      <c r="E187" s="12" t="s">
         <v>457</v>
       </c>
-      <c r="F187" s="20" t="s">
+      <c r="F187" s="19" t="s">
         <v>458</v>
       </c>
       <c r="G187" s="17" t="s">
@@ -7711,10 +7706,10 @@
       <c r="D188" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E188" s="19" t="s">
+      <c r="E188" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="F188" s="20" t="s">
+      <c r="F188" s="19" t="s">
         <v>461</v>
       </c>
       <c r="G188" s="17" t="s">
@@ -7737,7 +7732,7 @@
       <c r="D189" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E189" s="19" t="s">
+      <c r="E189" s="12" t="s">
         <v>464</v>
       </c>
       <c r="F189" s="13" t="s">
@@ -7763,10 +7758,10 @@
       <c r="D190" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E190" s="19" t="s">
+      <c r="E190" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="F190" s="20" t="s">
+      <c r="F190" s="19" t="s">
         <v>468</v>
       </c>
       <c r="G190" s="17" t="s">
@@ -7789,10 +7784,10 @@
       <c r="D191" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E191" s="19" t="s">
+      <c r="E191" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="F191" s="20" t="s">
+      <c r="F191" s="19" t="s">
         <v>441</v>
       </c>
       <c r="G191" s="17" t="s">
@@ -7815,10 +7810,10 @@
       <c r="D192" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E192" s="19" t="s">
+      <c r="E192" s="12" t="s">
         <v>473</v>
       </c>
-      <c r="F192" s="20" t="s">
+      <c r="F192" s="19" t="s">
         <v>474</v>
       </c>
       <c r="G192" s="17" t="s">
@@ -7841,10 +7836,10 @@
       <c r="D193" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E193" s="19" t="s">
+      <c r="E193" s="12" t="s">
         <v>477</v>
       </c>
-      <c r="F193" s="20" t="s">
+      <c r="F193" s="19" t="s">
         <v>474</v>
       </c>
       <c r="G193" s="17" t="s">
@@ -7867,10 +7862,10 @@
       <c r="D194" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E194" s="19" t="s">
+      <c r="E194" s="12" t="s">
         <v>479</v>
       </c>
-      <c r="F194" s="20" t="s">
+      <c r="F194" s="19" t="s">
         <v>446</v>
       </c>
       <c r="G194" s="17" t="s">
@@ -7893,10 +7888,10 @@
       <c r="D195" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E195" s="19" t="s">
+      <c r="E195" s="12" t="s">
         <v>481</v>
       </c>
-      <c r="F195" s="20" t="s">
+      <c r="F195" s="19" t="s">
         <v>482</v>
       </c>
       <c r="G195" s="17" t="s">
@@ -7919,10 +7914,10 @@
       <c r="D196" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E196" s="19" t="s">
+      <c r="E196" s="12" t="s">
         <v>484</v>
       </c>
-      <c r="F196" s="20" t="s">
+      <c r="F196" s="19" t="s">
         <v>50</v>
       </c>
       <c r="G196" s="17" t="s">
@@ -7945,10 +7940,10 @@
       <c r="D197" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E197" s="19" t="s">
+      <c r="E197" s="12" t="s">
         <v>486</v>
       </c>
-      <c r="F197" s="20" t="s">
+      <c r="F197" s="19" t="s">
         <v>433</v>
       </c>
       <c r="G197" s="17" t="s">
@@ -7971,10 +7966,10 @@
       <c r="D198" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E198" s="19" t="s">
+      <c r="E198" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="F198" s="20" t="s">
+      <c r="F198" s="19" t="s">
         <v>412</v>
       </c>
       <c r="G198" s="17" t="s">
@@ -7997,10 +7992,10 @@
       <c r="D199" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E199" s="19" t="s">
+      <c r="E199" s="12" t="s">
         <v>489</v>
       </c>
-      <c r="F199" s="20" t="s">
+      <c r="F199" s="19" t="s">
         <v>482</v>
       </c>
       <c r="G199" s="17" t="s">
@@ -8023,10 +8018,10 @@
       <c r="D200" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E200" s="19" t="s">
+      <c r="E200" s="12" t="s">
         <v>491</v>
       </c>
-      <c r="F200" s="20" t="s">
+      <c r="F200" s="19" t="s">
         <v>55</v>
       </c>
       <c r="G200" s="17" t="s">
@@ -8049,10 +8044,10 @@
       <c r="D201" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E201" s="19" t="s">
+      <c r="E201" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F201" s="20" t="s">
+      <c r="F201" s="19" t="s">
         <v>493</v>
       </c>
       <c r="G201" s="17" t="s">
@@ -8075,10 +8070,10 @@
       <c r="D202" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E202" s="19" t="s">
+      <c r="E202" s="12" t="s">
         <v>496</v>
       </c>
-      <c r="F202" s="20" t="s">
+      <c r="F202" s="19" t="s">
         <v>461</v>
       </c>
       <c r="G202" s="17" t="s">
@@ -8101,10 +8096,10 @@
       <c r="D203" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E203" s="19" t="s">
+      <c r="E203" s="12" t="s">
         <v>498</v>
       </c>
-      <c r="F203" s="20" t="s">
+      <c r="F203" s="19" t="s">
         <v>412</v>
       </c>
       <c r="G203" s="17" t="s">
@@ -8127,10 +8122,10 @@
       <c r="D204" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E204" s="19" t="s">
+      <c r="E204" s="12" t="s">
         <v>500</v>
       </c>
-      <c r="F204" s="20" t="s">
+      <c r="F204" s="19" t="s">
         <v>433</v>
       </c>
       <c r="G204" s="17" t="s">
@@ -8153,10 +8148,10 @@
       <c r="D205" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E205" s="19" t="s">
+      <c r="E205" s="12" t="s">
         <v>502</v>
       </c>
-      <c r="F205" s="20" t="s">
+      <c r="F205" s="19" t="s">
         <v>55</v>
       </c>
       <c r="G205" s="17" t="s">
@@ -8179,10 +8174,10 @@
       <c r="D206" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E206" s="19" t="s">
+      <c r="E206" s="12" t="s">
         <v>504</v>
       </c>
-      <c r="F206" s="20" t="s">
+      <c r="F206" s="19" t="s">
         <v>461</v>
       </c>
       <c r="G206" s="17" t="s">
@@ -8205,10 +8200,10 @@
       <c r="D207" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E207" s="19" t="s">
+      <c r="E207" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="F207" s="20" t="s">
+      <c r="F207" s="19" t="s">
         <v>474</v>
       </c>
       <c r="G207" s="17" t="s">
@@ -8231,10 +8226,10 @@
       <c r="D208" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E208" s="19" t="s">
+      <c r="E208" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F208" s="20" t="s">
+      <c r="F208" s="19" t="s">
         <v>59</v>
       </c>
       <c r="G208" s="17" t="s">
@@ -8257,10 +8252,10 @@
       <c r="D209" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E209" s="19" t="s">
+      <c r="E209" s="12" t="s">
         <v>508</v>
       </c>
-      <c r="F209" s="20" t="s">
+      <c r="F209" s="19" t="s">
         <v>68</v>
       </c>
       <c r="G209" s="17" t="s">
@@ -8283,10 +8278,10 @@
       <c r="D210" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E210" s="19" t="s">
+      <c r="E210" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F210" s="20" t="s">
+      <c r="F210" s="19" t="s">
         <v>55</v>
       </c>
       <c r="G210" s="17" t="s">
@@ -8309,10 +8304,10 @@
       <c r="D211" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E211" s="19" t="s">
+      <c r="E211" s="12" t="s">
         <v>511</v>
       </c>
-      <c r="F211" s="20" t="s">
+      <c r="F211" s="19" t="s">
         <v>68</v>
       </c>
       <c r="G211" s="17" t="s">
@@ -8335,10 +8330,10 @@
       <c r="D212" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E212" s="19" t="s">
+      <c r="E212" s="12" t="s">
         <v>513</v>
       </c>
-      <c r="F212" s="20" t="s">
+      <c r="F212" s="19" t="s">
         <v>276</v>
       </c>
       <c r="G212" s="17" t="s">
@@ -8361,10 +8356,10 @@
       <c r="D213" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E213" s="19" t="s">
+      <c r="E213" s="12" t="s">
         <v>515</v>
       </c>
-      <c r="F213" s="20" t="s">
+      <c r="F213" s="19" t="s">
         <v>59</v>
       </c>
       <c r="G213" s="17" t="s">
@@ -8387,10 +8382,10 @@
       <c r="D214" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E214" s="19" t="s">
+      <c r="E214" s="12" t="s">
         <v>517</v>
       </c>
-      <c r="F214" s="20" t="s">
+      <c r="F214" s="19" t="s">
         <v>59</v>
       </c>
       <c r="G214" s="17" t="s">
@@ -8413,10 +8408,10 @@
       <c r="D215" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E215" s="19" t="s">
+      <c r="E215" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="F215" s="20" t="s">
+      <c r="F215" s="19" t="s">
         <v>412</v>
       </c>
       <c r="G215" s="17" t="s">
@@ -8439,10 +8434,10 @@
       <c r="D216" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E216" s="19" t="s">
+      <c r="E216" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F216" s="20" t="s">
+      <c r="F216" s="19" t="s">
         <v>441</v>
       </c>
       <c r="G216" s="17" t="s">
@@ -8465,10 +8460,10 @@
       <c r="D217" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E217" s="19" t="s">
+      <c r="E217" s="12" t="s">
         <v>521</v>
       </c>
-      <c r="F217" s="20" t="s">
+      <c r="F217" s="19" t="s">
         <v>55</v>
       </c>
       <c r="G217" s="17" t="s">
@@ -8491,10 +8486,10 @@
       <c r="D218" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E218" s="19" t="s">
+      <c r="E218" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="F218" s="20" t="s">
+      <c r="F218" s="19" t="s">
         <v>59</v>
       </c>
       <c r="G218" s="17" t="s">
@@ -8517,10 +8512,10 @@
       <c r="D219" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E219" s="19" t="s">
+      <c r="E219" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="F219" s="20" t="s">
+      <c r="F219" s="19" t="s">
         <v>458</v>
       </c>
       <c r="G219" s="17" t="s">
@@ -8543,10 +8538,10 @@
       <c r="D220" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E220" s="19" t="s">
+      <c r="E220" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="F220" s="20" t="s">
+      <c r="F220" s="19" t="s">
         <v>525</v>
       </c>
       <c r="G220" s="17" t="s">
@@ -8569,10 +8564,10 @@
       <c r="D221" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E221" s="19" t="s">
+      <c r="E221" s="12" t="s">
         <v>527</v>
       </c>
-      <c r="F221" s="20" t="s">
+      <c r="F221" s="19" t="s">
         <v>276</v>
       </c>
       <c r="G221" s="17" t="s">
@@ -8595,10 +8590,10 @@
       <c r="D222" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E222" s="19" t="s">
+      <c r="E222" s="12" t="s">
         <v>529</v>
       </c>
-      <c r="F222" s="20" t="s">
+      <c r="F222" s="19" t="s">
         <v>55</v>
       </c>
       <c r="G222" s="17" t="s">
@@ -8621,10 +8616,10 @@
       <c r="D223" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E223" s="19" t="s">
+      <c r="E223" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="F223" s="20" t="s">
+      <c r="F223" s="19" t="s">
         <v>441</v>
       </c>
       <c r="G223" s="17" t="s">
@@ -8647,10 +8642,10 @@
       <c r="D224" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E224" s="19" t="s">
+      <c r="E224" s="12" t="s">
         <v>532</v>
       </c>
-      <c r="F224" s="20" t="s">
+      <c r="F224" s="19" t="s">
         <v>276</v>
       </c>
       <c r="G224" s="17" t="s">
@@ -8673,10 +8668,10 @@
       <c r="D225" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E225" s="19" t="s">
+      <c r="E225" s="12" t="s">
         <v>534</v>
       </c>
-      <c r="F225" s="20" t="s">
+      <c r="F225" s="19" t="s">
         <v>59</v>
       </c>
       <c r="G225" s="17" t="s">
@@ -8699,10 +8694,10 @@
       <c r="D226" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E226" s="19" t="s">
+      <c r="E226" s="12" t="s">
         <v>536</v>
       </c>
-      <c r="F226" s="20" t="s">
+      <c r="F226" s="19" t="s">
         <v>276</v>
       </c>
       <c r="G226" s="17" t="s">
@@ -8725,10 +8720,10 @@
       <c r="D227" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E227" s="19" t="s">
+      <c r="E227" s="12" t="s">
         <v>538</v>
       </c>
-      <c r="F227" s="20" t="s">
+      <c r="F227" s="19" t="s">
         <v>493</v>
       </c>
       <c r="G227" s="17" t="s">
@@ -8751,10 +8746,10 @@
       <c r="D228" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E228" s="19" t="s">
+      <c r="E228" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="F228" s="20" t="s">
+      <c r="F228" s="19" t="s">
         <v>441</v>
       </c>
       <c r="G228" s="17" t="s">
@@ -8777,10 +8772,10 @@
       <c r="D229" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E229" s="19" t="s">
+      <c r="E229" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="F229" s="20" t="s">
+      <c r="F229" s="19" t="s">
         <v>412</v>
       </c>
       <c r="G229" s="17" t="s">
@@ -8803,10 +8798,10 @@
       <c r="D230" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E230" s="19" t="s">
+      <c r="E230" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F230" s="20" t="s">
+      <c r="F230" s="19" t="s">
         <v>50</v>
       </c>
       <c r="G230" s="17" t="s">
@@ -8829,10 +8824,10 @@
       <c r="D231" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E231" s="19" t="s">
+      <c r="E231" s="12" t="s">
         <v>544</v>
       </c>
-      <c r="F231" s="20" t="s">
+      <c r="F231" s="19" t="s">
         <v>461</v>
       </c>
       <c r="G231" s="17" t="s">
@@ -8855,10 +8850,10 @@
       <c r="D232" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E232" s="19" t="s">
+      <c r="E232" s="12" t="s">
         <v>546</v>
       </c>
-      <c r="F232" s="20" t="s">
+      <c r="F232" s="19" t="s">
         <v>474</v>
       </c>
       <c r="G232" s="17" t="s">
@@ -8881,10 +8876,10 @@
       <c r="D233" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E233" s="19" t="s">
+      <c r="E233" s="12" t="s">
         <v>548</v>
       </c>
-      <c r="F233" s="20" t="s">
+      <c r="F233" s="19" t="s">
         <v>461</v>
       </c>
       <c r="G233" s="17" t="s">
@@ -8907,10 +8902,10 @@
       <c r="D234" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E234" s="19" t="s">
+      <c r="E234" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="F234" s="20" t="s">
+      <c r="F234" s="19" t="s">
         <v>59</v>
       </c>
       <c r="G234" s="17" t="s">
@@ -8927,22 +8922,22 @@
       <c r="B235" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C235" s="24" t="s">
+      <c r="C235" s="23" t="s">
         <v>550</v>
       </c>
       <c r="D235" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E235" s="25" t="s">
+      <c r="E235" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="F235" s="26" t="s">
+      <c r="F235" s="25" t="s">
         <v>551</v>
       </c>
-      <c r="G235" s="24" t="s">
+      <c r="G235" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="H235" s="24" t="s">
+      <c r="H235" s="23" t="s">
         <v>552</v>
       </c>
     </row>
@@ -8953,22 +8948,22 @@
       <c r="B236" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C236" s="24" t="s">
+      <c r="C236" s="23" t="s">
         <v>553</v>
       </c>
       <c r="D236" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E236" s="25" t="s">
+      <c r="E236" s="24" t="s">
         <v>554</v>
       </c>
-      <c r="F236" s="26" t="s">
+      <c r="F236" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="G236" s="24" t="s">
+      <c r="G236" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="H236" s="24" t="s">
+      <c r="H236" s="23" t="s">
         <v>100</v>
       </c>
     </row>
@@ -8979,22 +8974,22 @@
       <c r="B237" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C237" s="24" t="s">
+      <c r="C237" s="23" t="s">
         <v>555</v>
       </c>
       <c r="D237" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E237" s="25" t="s">
+      <c r="E237" s="24" t="s">
         <v>556</v>
       </c>
-      <c r="F237" s="26" t="s">
+      <c r="F237" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="G237" s="24" t="s">
+      <c r="G237" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="H237" s="24" t="s">
+      <c r="H237" s="23" t="s">
         <v>100</v>
       </c>
     </row>
@@ -9005,22 +9000,22 @@
       <c r="B238" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C238" s="24" t="s">
+      <c r="C238" s="23" t="s">
         <v>557</v>
       </c>
       <c r="D238" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E238" s="25" t="s">
+      <c r="E238" s="24" t="s">
         <v>558</v>
       </c>
-      <c r="F238" s="26" t="s">
+      <c r="F238" s="25" t="s">
         <v>559</v>
       </c>
-      <c r="G238" s="24" t="s">
+      <c r="G238" s="23" t="s">
         <v>559</v>
       </c>
-      <c r="H238" s="24" t="s">
+      <c r="H238" s="23" t="s">
         <v>560</v>
       </c>
     </row>
@@ -9031,22 +9026,22 @@
       <c r="B239" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C239" s="24" t="s">
+      <c r="C239" s="23" t="s">
         <v>561</v>
       </c>
       <c r="D239" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E239" s="25" t="s">
+      <c r="E239" s="24" t="s">
         <v>562</v>
       </c>
-      <c r="F239" s="26" t="s">
+      <c r="F239" s="25" t="s">
         <v>551</v>
       </c>
-      <c r="G239" s="24" t="s">
+      <c r="G239" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="H239" s="24" t="s">
+      <c r="H239" s="23" t="s">
         <v>552</v>
       </c>
     </row>
@@ -9057,22 +9052,22 @@
       <c r="B240" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C240" s="24" t="s">
+      <c r="C240" s="23" t="s">
         <v>563</v>
       </c>
       <c r="D240" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E240" s="25" t="s">
+      <c r="E240" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="F240" s="26" t="s">
+      <c r="F240" s="25" t="s">
         <v>564</v>
       </c>
-      <c r="G240" s="24" t="s">
+      <c r="G240" s="23" t="s">
         <v>565</v>
       </c>
-      <c r="H240" s="24" t="s">
+      <c r="H240" s="23" t="s">
         <v>566</v>
       </c>
     </row>
@@ -9083,22 +9078,22 @@
       <c r="B241" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C241" s="24" t="s">
+      <c r="C241" s="23" t="s">
         <v>567</v>
       </c>
       <c r="D241" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E241" s="25" t="s">
+      <c r="E241" s="24" t="s">
         <v>568</v>
       </c>
-      <c r="F241" s="26" t="s">
+      <c r="F241" s="25" t="s">
         <v>551</v>
       </c>
-      <c r="G241" s="24" t="s">
+      <c r="G241" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="H241" s="24" t="s">
+      <c r="H241" s="23" t="s">
         <v>552</v>
       </c>
     </row>
@@ -9109,22 +9104,22 @@
       <c r="B242" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C242" s="24" t="s">
+      <c r="C242" s="23" t="s">
         <v>569</v>
       </c>
       <c r="D242" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E242" s="25" t="s">
+      <c r="E242" s="24" t="s">
         <v>570</v>
       </c>
-      <c r="F242" s="26" t="s">
+      <c r="F242" s="25" t="s">
         <v>559</v>
       </c>
-      <c r="G242" s="24" t="s">
+      <c r="G242" s="23" t="s">
         <v>559</v>
       </c>
-      <c r="H242" s="24" t="s">
+      <c r="H242" s="23" t="s">
         <v>560</v>
       </c>
     </row>
@@ -9135,22 +9130,22 @@
       <c r="B243" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C243" s="24" t="s">
+      <c r="C243" s="23" t="s">
         <v>571</v>
       </c>
       <c r="D243" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E243" s="25" t="s">
+      <c r="E243" s="24" t="s">
         <v>572</v>
       </c>
-      <c r="F243" s="26" t="s">
+      <c r="F243" s="25" t="s">
         <v>551</v>
       </c>
-      <c r="G243" s="24" t="s">
+      <c r="G243" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="H243" s="24" t="s">
+      <c r="H243" s="23" t="s">
         <v>552</v>
       </c>
     </row>
@@ -9161,22 +9156,22 @@
       <c r="B244" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C244" s="24" t="s">
+      <c r="C244" s="23" t="s">
         <v>573</v>
       </c>
       <c r="D244" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E244" s="25" t="s">
+      <c r="E244" s="24" t="s">
         <v>574</v>
       </c>
-      <c r="F244" s="26" t="s">
+      <c r="F244" s="25" t="s">
         <v>564</v>
       </c>
-      <c r="G244" s="24" t="s">
+      <c r="G244" s="23" t="s">
         <v>565</v>
       </c>
-      <c r="H244" s="24" t="s">
+      <c r="H244" s="23" t="s">
         <v>566</v>
       </c>
     </row>
@@ -9187,22 +9182,22 @@
       <c r="B245" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C245" s="24" t="s">
+      <c r="C245" s="23" t="s">
         <v>575</v>
       </c>
       <c r="D245" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E245" s="25" t="s">
+      <c r="E245" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="F245" s="26" t="s">
+      <c r="F245" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="G245" s="24" t="s">
+      <c r="G245" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H245" s="24" t="s">
+      <c r="H245" s="23" t="s">
         <v>576</v>
       </c>
     </row>
@@ -9213,22 +9208,22 @@
       <c r="B246" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C246" s="24" t="s">
+      <c r="C246" s="23" t="s">
         <v>577</v>
       </c>
       <c r="D246" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E246" s="25" t="s">
+      <c r="E246" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F246" s="26" t="s">
+      <c r="F246" s="25" t="s">
         <v>564</v>
       </c>
-      <c r="G246" s="24" t="s">
+      <c r="G246" s="23" t="s">
         <v>565</v>
       </c>
-      <c r="H246" s="24" t="s">
+      <c r="H246" s="23" t="s">
         <v>566</v>
       </c>
     </row>
@@ -9239,22 +9234,22 @@
       <c r="B247" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C247" s="23" t="s">
+      <c r="C247" s="22" t="s">
         <v>578</v>
       </c>
       <c r="D247" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E247" s="27" t="s">
+      <c r="E247" s="26" t="s">
         <v>579</v>
       </c>
-      <c r="F247" s="23" t="s">
+      <c r="F247" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G247" s="23" t="s">
+      <c r="G247" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H247" s="23" t="s">
+      <c r="H247" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -9265,22 +9260,22 @@
       <c r="B248" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C248" s="23" t="s">
+      <c r="C248" s="22" t="s">
         <v>580</v>
       </c>
       <c r="D248" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E248" s="27" t="s">
+      <c r="E248" s="26" t="s">
         <v>581</v>
       </c>
-      <c r="F248" s="23" t="s">
+      <c r="F248" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G248" s="23" t="s">
+      <c r="G248" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H248" s="23" t="s">
+      <c r="H248" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -9291,22 +9286,22 @@
       <c r="B249" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C249" s="23" t="s">
+      <c r="C249" s="22" t="s">
         <v>584</v>
       </c>
       <c r="D249" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E249" s="27" t="s">
+      <c r="E249" s="26" t="s">
         <v>585</v>
       </c>
-      <c r="F249" s="23" t="s">
+      <c r="F249" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G249" s="23" t="s">
+      <c r="G249" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H249" s="23" t="s">
+      <c r="H249" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -9317,22 +9312,22 @@
       <c r="B250" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C250" s="23" t="s">
+      <c r="C250" s="22" t="s">
         <v>586</v>
       </c>
       <c r="D250" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E250" s="27" t="s">
+      <c r="E250" s="26" t="s">
         <v>587</v>
       </c>
-      <c r="F250" s="23" t="s">
+      <c r="F250" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G250" s="23" t="s">
+      <c r="G250" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H250" s="23" t="s">
+      <c r="H250" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -9343,22 +9338,22 @@
       <c r="B251" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C251" s="23" t="s">
+      <c r="C251" s="22" t="s">
         <v>588</v>
       </c>
       <c r="D251" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E251" s="27" t="s">
+      <c r="E251" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="F251" s="23" t="s">
+      <c r="F251" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G251" s="23" t="s">
+      <c r="G251" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H251" s="23" t="s">
+      <c r="H251" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -9369,22 +9364,22 @@
       <c r="B252" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C252" s="23" t="s">
+      <c r="C252" s="22" t="s">
         <v>589</v>
       </c>
       <c r="D252" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E252" s="27" t="s">
+      <c r="E252" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="F252" s="23" t="s">
+      <c r="F252" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G252" s="23" t="s">
+      <c r="G252" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H252" s="23" t="s">
+      <c r="H252" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -9395,22 +9390,22 @@
       <c r="B253" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C253" s="23" t="s">
+      <c r="C253" s="22" t="s">
         <v>590</v>
       </c>
       <c r="D253" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E253" s="27" t="s">
+      <c r="E253" s="26" t="s">
         <v>591</v>
       </c>
-      <c r="F253" s="23" t="s">
+      <c r="F253" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G253" s="23" t="s">
+      <c r="G253" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H253" s="23" t="s">
+      <c r="H253" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -9421,22 +9416,22 @@
       <c r="B254" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C254" s="23" t="s">
+      <c r="C254" s="22" t="s">
         <v>592</v>
       </c>
       <c r="D254" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E254" s="27">
+      <c r="E254" s="26">
         <v>142</v>
       </c>
-      <c r="F254" s="23" t="s">
+      <c r="F254" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G254" s="23" t="s">
+      <c r="G254" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H254" s="23" t="s">
+      <c r="H254" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -9447,22 +9442,22 @@
       <c r="B255" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C255" s="23" t="s">
+      <c r="C255" s="22" t="s">
         <v>593</v>
       </c>
       <c r="D255" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E255" s="27" t="s">
+      <c r="E255" s="26" t="s">
         <v>594</v>
       </c>
-      <c r="F255" s="23" t="s">
+      <c r="F255" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G255" s="23" t="s">
+      <c r="G255" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H255" s="23" t="s">
+      <c r="H255" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -9473,1352 +9468,1352 @@
       <c r="B256" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C256" s="23" t="s">
+      <c r="C256" s="22" t="s">
         <v>595</v>
       </c>
       <c r="D256" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E256" s="27" t="s">
+      <c r="E256" s="26" t="s">
         <v>596</v>
       </c>
-      <c r="F256" s="23" t="s">
+      <c r="F256" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G256" s="23" t="s">
+      <c r="G256" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H256" s="23" t="s">
+      <c r="H256" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="257" ht="14.25">
+    <row r="257" ht="42.75">
       <c r="A257" s="5">
         <v>256</v>
       </c>
       <c r="B257" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C257" s="23" t="s">
+      <c r="C257" s="22" t="s">
         <v>597</v>
       </c>
       <c r="D257" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E257" s="27" t="s">
+      <c r="E257" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="F257" s="23" t="s">
+      <c r="F257" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G257" s="23" t="s">
+      <c r="G257" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H257" s="23" t="s">
+      <c r="H257" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="258" ht="14.25">
+    <row r="258" ht="42.75">
       <c r="A258" s="5">
         <v>257</v>
       </c>
       <c r="B258" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C258" s="23" t="s">
+      <c r="C258" s="22" t="s">
         <v>598</v>
       </c>
       <c r="D258" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E258" s="27" t="s">
+      <c r="E258" s="26" t="s">
         <v>599</v>
       </c>
-      <c r="F258" s="23" t="s">
+      <c r="F258" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G258" s="23" t="s">
+      <c r="G258" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H258" s="23" t="s">
+      <c r="H258" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="259" ht="14.25">
+    <row r="259" ht="42.75">
       <c r="A259" s="5">
         <v>258</v>
       </c>
       <c r="B259" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C259" s="23" t="s">
+      <c r="C259" s="22" t="s">
         <v>600</v>
       </c>
       <c r="D259" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E259" s="27" t="s">
+      <c r="E259" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="F259" s="23" t="s">
+      <c r="F259" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G259" s="23" t="s">
+      <c r="G259" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H259" s="23" t="s">
+      <c r="H259" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="260" ht="14.25">
+    <row r="260" ht="42.75">
       <c r="A260" s="5">
         <v>259</v>
       </c>
       <c r="B260" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C260" s="23" t="s">
+      <c r="C260" s="22" t="s">
         <v>601</v>
       </c>
       <c r="D260" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E260" s="27" t="s">
+      <c r="E260" s="26" t="s">
         <v>602</v>
       </c>
-      <c r="F260" s="23" t="s">
+      <c r="F260" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G260" s="23" t="s">
+      <c r="G260" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H260" s="23" t="s">
+      <c r="H260" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="261" ht="14.25">
+    <row r="261" ht="42.75">
       <c r="A261" s="5">
         <v>260</v>
       </c>
       <c r="B261" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C261" s="23" t="s">
+      <c r="C261" s="22" t="s">
         <v>603</v>
       </c>
       <c r="D261" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E261" s="27" t="s">
+      <c r="E261" s="26" t="s">
         <v>604</v>
       </c>
-      <c r="F261" s="23" t="s">
+      <c r="F261" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G261" s="23" t="s">
+      <c r="G261" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H261" s="23" t="s">
+      <c r="H261" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="262" ht="14.25">
+    <row r="262" ht="42.75">
       <c r="A262" s="5">
         <v>261</v>
       </c>
       <c r="B262" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C262" s="23" t="s">
+      <c r="C262" s="22" t="s">
         <v>605</v>
       </c>
       <c r="D262" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E262" s="27" t="s">
+      <c r="E262" s="26" t="s">
         <v>440</v>
       </c>
-      <c r="F262" s="23" t="s">
+      <c r="F262" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G262" s="23" t="s">
+      <c r="G262" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H262" s="23" t="s">
+      <c r="H262" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="263" ht="14.25">
+    <row r="263" ht="42.75">
       <c r="A263" s="5">
         <v>262</v>
       </c>
       <c r="B263" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C263" s="23" t="s">
+      <c r="C263" s="22" t="s">
         <v>606</v>
       </c>
       <c r="D263" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E263" s="27" t="s">
+      <c r="E263" s="26" t="s">
         <v>607</v>
       </c>
-      <c r="F263" s="23" t="s">
+      <c r="F263" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G263" s="23" t="s">
+      <c r="G263" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H263" s="23" t="s">
+      <c r="H263" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="264" ht="14.25">
+    <row r="264" ht="42.75">
       <c r="A264" s="5">
         <v>263</v>
       </c>
       <c r="B264" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C264" s="23" t="s">
+      <c r="C264" s="22" t="s">
         <v>608</v>
       </c>
       <c r="D264" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E264" s="27" t="s">
+      <c r="E264" s="26" t="s">
         <v>609</v>
       </c>
-      <c r="F264" s="23" t="s">
+      <c r="F264" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G264" s="23" t="s">
+      <c r="G264" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H264" s="23" t="s">
+      <c r="H264" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="265" ht="14.25">
+    <row r="265" ht="42.75">
       <c r="A265" s="5">
         <v>264</v>
       </c>
       <c r="B265" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C265" s="23" t="s">
+      <c r="C265" s="22" t="s">
         <v>610</v>
       </c>
       <c r="D265" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E265" s="27" t="s">
+      <c r="E265" s="26" t="s">
         <v>611</v>
       </c>
-      <c r="F265" s="23" t="s">
+      <c r="F265" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G265" s="23" t="s">
+      <c r="G265" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H265" s="23" t="s">
+      <c r="H265" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="266" ht="14.25">
+    <row r="266" ht="42.75">
       <c r="A266" s="5">
         <v>265</v>
       </c>
       <c r="B266" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C266" s="23" t="s">
+      <c r="C266" s="22" t="s">
         <v>612</v>
       </c>
       <c r="D266" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E266" s="27" t="s">
+      <c r="E266" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="F266" s="23" t="s">
+      <c r="F266" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G266" s="23" t="s">
+      <c r="G266" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H266" s="23" t="s">
+      <c r="H266" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="267" ht="14.25">
+    <row r="267" ht="42.75">
       <c r="A267" s="5">
         <v>266</v>
       </c>
       <c r="B267" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C267" s="23" t="s">
+      <c r="C267" s="22" t="s">
         <v>613</v>
       </c>
       <c r="D267" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E267" s="27" t="s">
+      <c r="E267" s="26" t="s">
         <v>614</v>
       </c>
-      <c r="F267" s="23" t="s">
+      <c r="F267" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G267" s="23" t="s">
+      <c r="G267" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H267" s="23" t="s">
+      <c r="H267" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="268" ht="14.25">
+    <row r="268" ht="42.75">
       <c r="A268" s="5">
         <v>267</v>
       </c>
       <c r="B268" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C268" s="28" t="s">
+      <c r="C268" s="27" t="s">
         <v>615</v>
       </c>
       <c r="D268" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E268" s="29" t="s">
+      <c r="E268" s="28" t="s">
         <v>616</v>
       </c>
-      <c r="F268" s="28" t="s">
+      <c r="F268" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="G268" s="28" t="s">
+      <c r="G268" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="H268" s="28" t="s">
+      <c r="H268" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="269" ht="14.25">
+    <row r="269" ht="42.75">
       <c r="A269" s="5">
         <v>268</v>
       </c>
       <c r="B269" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C269" s="23" t="s">
+      <c r="C269" s="22" t="s">
         <v>617</v>
       </c>
       <c r="D269" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E269" s="27" t="s">
+      <c r="E269" s="26" t="s">
         <v>618</v>
       </c>
-      <c r="F269" s="23" t="s">
+      <c r="F269" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G269" s="23" t="s">
+      <c r="G269" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H269" s="23" t="s">
+      <c r="H269" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="270" ht="14.25">
+    <row r="270" ht="42.75">
       <c r="A270" s="5">
         <v>269</v>
       </c>
       <c r="B270" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C270" s="23" t="s">
+      <c r="C270" s="22" t="s">
         <v>619</v>
       </c>
       <c r="D270" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E270" s="27" t="s">
+      <c r="E270" s="26" t="s">
         <v>620</v>
       </c>
-      <c r="F270" s="23" t="s">
+      <c r="F270" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G270" s="23" t="s">
+      <c r="G270" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H270" s="23" t="s">
+      <c r="H270" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="271" ht="14.25">
+    <row r="271" ht="42.75">
       <c r="A271" s="5">
         <v>270</v>
       </c>
       <c r="B271" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C271" s="23" t="s">
+      <c r="C271" s="22" t="s">
         <v>621</v>
       </c>
       <c r="D271" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E271" s="27" t="s">
+      <c r="E271" s="26" t="s">
         <v>622</v>
       </c>
-      <c r="F271" s="23" t="s">
+      <c r="F271" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G271" s="23" t="s">
+      <c r="G271" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H271" s="23" t="s">
+      <c r="H271" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="272" ht="14.25">
+    <row r="272" ht="42.75">
       <c r="A272" s="5">
         <v>271</v>
       </c>
       <c r="B272" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C272" s="23" t="s">
+      <c r="C272" s="22" t="s">
         <v>623</v>
       </c>
       <c r="D272" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E272" s="27" t="s">
+      <c r="E272" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="F272" s="23" t="s">
+      <c r="F272" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G272" s="23" t="s">
+      <c r="G272" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H272" s="23" t="s">
+      <c r="H272" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="273" ht="14.25">
+    <row r="273" ht="42.75">
       <c r="A273" s="5">
         <v>272</v>
       </c>
       <c r="B273" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C273" s="28" t="s">
+      <c r="C273" s="27" t="s">
         <v>624</v>
       </c>
       <c r="D273" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E273" s="27" t="s">
+      <c r="E273" s="26" t="s">
         <v>625</v>
       </c>
-      <c r="F273" s="28" t="s">
+      <c r="F273" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="G273" s="28" t="s">
+      <c r="G273" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="H273" s="28" t="s">
+      <c r="H273" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="274" ht="14.25">
+    <row r="274" ht="42.75">
       <c r="A274" s="5">
         <v>273</v>
       </c>
       <c r="B274" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C274" s="23" t="s">
+      <c r="C274" s="22" t="s">
         <v>626</v>
       </c>
       <c r="D274" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E274" s="27" t="s">
+      <c r="E274" s="26" t="s">
         <v>627</v>
       </c>
-      <c r="F274" s="23" t="s">
+      <c r="F274" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G274" s="23" t="s">
+      <c r="G274" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H274" s="23" t="s">
+      <c r="H274" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="275" ht="14.25">
+    <row r="275" ht="42.75">
       <c r="A275" s="5">
         <v>274</v>
       </c>
       <c r="B275" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C275" s="23" t="s">
+      <c r="C275" s="22" t="s">
         <v>628</v>
       </c>
       <c r="D275" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E275" s="27" t="s">
+      <c r="E275" s="26" t="s">
         <v>629</v>
       </c>
-      <c r="F275" s="23" t="s">
+      <c r="F275" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G275" s="23" t="s">
+      <c r="G275" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H275" s="23" t="s">
+      <c r="H275" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="276" ht="14.25">
+    <row r="276" ht="42.75">
       <c r="A276" s="5">
         <v>275</v>
       </c>
       <c r="B276" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C276" s="23" t="s">
+      <c r="C276" s="22" t="s">
         <v>630</v>
       </c>
       <c r="D276" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E276" s="27" t="s">
+      <c r="E276" s="26" t="s">
         <v>631</v>
       </c>
-      <c r="F276" s="23" t="s">
+      <c r="F276" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G276" s="23" t="s">
+      <c r="G276" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H276" s="23" t="s">
+      <c r="H276" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="277" ht="14.25">
+    <row r="277" ht="42.75">
       <c r="A277" s="5">
         <v>276</v>
       </c>
       <c r="B277" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C277" s="23" t="s">
+      <c r="C277" s="22" t="s">
         <v>632</v>
       </c>
       <c r="D277" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E277" s="27" t="s">
+      <c r="E277" s="26" t="s">
         <v>633</v>
       </c>
-      <c r="F277" s="23" t="s">
+      <c r="F277" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G277" s="23" t="s">
+      <c r="G277" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H277" s="23" t="s">
+      <c r="H277" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="278" ht="14.25">
+    <row r="278" ht="42.75">
       <c r="A278" s="5">
         <v>277</v>
       </c>
       <c r="B278" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C278" s="23" t="s">
+      <c r="C278" s="22" t="s">
         <v>634</v>
       </c>
       <c r="D278" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E278" s="27" t="s">
+      <c r="E278" s="26" t="s">
         <v>635</v>
       </c>
-      <c r="F278" s="23" t="s">
+      <c r="F278" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G278" s="23" t="s">
+      <c r="G278" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H278" s="23" t="s">
+      <c r="H278" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="279" ht="14.25">
+    <row r="279" ht="42.75">
       <c r="A279" s="5">
         <v>278</v>
       </c>
       <c r="B279" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C279" s="23" t="s">
+      <c r="C279" s="22" t="s">
         <v>636</v>
       </c>
       <c r="D279" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E279" s="27" t="s">
+      <c r="E279" s="26" t="s">
         <v>637</v>
       </c>
-      <c r="F279" s="23" t="s">
+      <c r="F279" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G279" s="23" t="s">
+      <c r="G279" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H279" s="23" t="s">
+      <c r="H279" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="280" ht="14.25">
+    <row r="280" ht="42.75">
       <c r="A280" s="5">
         <v>279</v>
       </c>
       <c r="B280" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C280" s="23" t="s">
+      <c r="C280" s="22" t="s">
         <v>638</v>
       </c>
       <c r="D280" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E280" s="27" t="s">
+      <c r="E280" s="26" t="s">
         <v>639</v>
       </c>
-      <c r="F280" s="23" t="s">
+      <c r="F280" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G280" s="23" t="s">
+      <c r="G280" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H280" s="23" t="s">
+      <c r="H280" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="281" ht="14.25">
+    <row r="281" ht="42.75">
       <c r="A281" s="5">
         <v>280</v>
       </c>
       <c r="B281" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C281" s="23" t="s">
+      <c r="C281" s="22" t="s">
         <v>640</v>
       </c>
       <c r="D281" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E281" s="27" t="s">
+      <c r="E281" s="26" t="s">
         <v>641</v>
       </c>
-      <c r="F281" s="23" t="s">
+      <c r="F281" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G281" s="23" t="s">
+      <c r="G281" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H281" s="23" t="s">
+      <c r="H281" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="282" ht="14.25">
+    <row r="282" ht="42.75">
       <c r="A282" s="5">
         <v>281</v>
       </c>
       <c r="B282" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C282" s="23" t="s">
+      <c r="C282" s="22" t="s">
         <v>642</v>
       </c>
       <c r="D282" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E282" s="27" t="s">
+      <c r="E282" s="26" t="s">
         <v>643</v>
       </c>
-      <c r="F282" s="23" t="s">
+      <c r="F282" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G282" s="23" t="s">
+      <c r="G282" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H282" s="23" t="s">
+      <c r="H282" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="283" ht="14.25">
+    <row r="283" ht="42.75">
       <c r="A283" s="5">
         <v>282</v>
       </c>
       <c r="B283" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C283" s="23" t="s">
+      <c r="C283" s="22" t="s">
         <v>644</v>
       </c>
       <c r="D283" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E283" s="27" t="s">
+      <c r="E283" s="26" t="s">
         <v>645</v>
       </c>
-      <c r="F283" s="23" t="s">
+      <c r="F283" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G283" s="23" t="s">
+      <c r="G283" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H283" s="23" t="s">
+      <c r="H283" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="284" ht="14.25">
+    <row r="284" ht="42.75">
       <c r="A284" s="5">
         <v>283</v>
       </c>
       <c r="B284" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C284" s="23" t="s">
+      <c r="C284" s="22" t="s">
         <v>646</v>
       </c>
       <c r="D284" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E284" s="27" t="s">
+      <c r="E284" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="F284" s="23" t="s">
+      <c r="F284" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G284" s="23" t="s">
+      <c r="G284" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H284" s="23" t="s">
+      <c r="H284" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="285" ht="14.25">
+    <row r="285" ht="42.75">
       <c r="A285" s="5">
         <v>284</v>
       </c>
       <c r="B285" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C285" s="23" t="s">
+      <c r="C285" s="22" t="s">
         <v>647</v>
       </c>
       <c r="D285" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E285" s="27" t="s">
+      <c r="E285" s="26" t="s">
         <v>648</v>
       </c>
-      <c r="F285" s="23" t="s">
+      <c r="F285" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G285" s="23" t="s">
+      <c r="G285" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H285" s="23" t="s">
+      <c r="H285" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="286" ht="14.25">
+    <row r="286" ht="42.75">
       <c r="A286" s="5">
         <v>285</v>
       </c>
       <c r="B286" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C286" s="23" t="s">
+      <c r="C286" s="22" t="s">
         <v>649</v>
       </c>
       <c r="D286" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E286" s="27" t="s">
+      <c r="E286" s="26" t="s">
         <v>650</v>
       </c>
-      <c r="F286" s="23" t="s">
+      <c r="F286" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G286" s="23" t="s">
+      <c r="G286" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H286" s="23" t="s">
+      <c r="H286" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="287" ht="14.25">
+    <row r="287" ht="42.75">
       <c r="A287" s="5">
         <v>286</v>
       </c>
       <c r="B287" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C287" s="23" t="s">
+      <c r="C287" s="22" t="s">
         <v>651</v>
       </c>
       <c r="D287" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E287" s="27" t="s">
+      <c r="E287" s="26" t="s">
         <v>652</v>
       </c>
-      <c r="F287" s="23" t="s">
+      <c r="F287" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G287" s="23" t="s">
+      <c r="G287" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H287" s="23" t="s">
+      <c r="H287" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="288" ht="14.25">
+    <row r="288" ht="42.75">
       <c r="A288" s="5">
         <v>287</v>
       </c>
       <c r="B288" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C288" s="23" t="s">
+      <c r="C288" s="22" t="s">
         <v>653</v>
       </c>
       <c r="D288" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E288" s="27" t="s">
+      <c r="E288" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="F288" s="23" t="s">
+      <c r="F288" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G288" s="23" t="s">
+      <c r="G288" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H288" s="23" t="s">
+      <c r="H288" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="289" ht="14.25">
+    <row r="289" ht="42.75">
       <c r="A289" s="5">
         <v>288</v>
       </c>
       <c r="B289" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C289" s="23" t="s">
+      <c r="C289" s="22" t="s">
         <v>654</v>
       </c>
       <c r="D289" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E289" s="27" t="s">
+      <c r="E289" s="26" t="s">
         <v>655</v>
       </c>
-      <c r="F289" s="23" t="s">
+      <c r="F289" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G289" s="23" t="s">
+      <c r="G289" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H289" s="23" t="s">
+      <c r="H289" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="290" ht="14.25">
+    <row r="290" ht="42.75">
       <c r="A290" s="5">
         <v>289</v>
       </c>
       <c r="B290" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C290" s="23" t="s">
+      <c r="C290" s="22" t="s">
         <v>656</v>
       </c>
       <c r="D290" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E290" s="27" t="s">
+      <c r="E290" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="F290" s="23" t="s">
+      <c r="F290" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G290" s="23" t="s">
+      <c r="G290" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H290" s="23" t="s">
+      <c r="H290" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="291" ht="14.25">
+    <row r="291" ht="42.75">
       <c r="A291" s="5">
         <v>290</v>
       </c>
       <c r="B291" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C291" s="23" t="s">
+      <c r="C291" s="22" t="s">
         <v>657</v>
       </c>
       <c r="D291" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E291" s="27" t="s">
+      <c r="E291" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="F291" s="23" t="s">
+      <c r="F291" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G291" s="23" t="s">
+      <c r="G291" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H291" s="23" t="s">
+      <c r="H291" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="292" ht="14.25">
+    <row r="292" ht="42.75">
       <c r="A292" s="5">
         <v>291</v>
       </c>
       <c r="B292" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C292" s="23" t="s">
+      <c r="C292" s="22" t="s">
         <v>658</v>
       </c>
       <c r="D292" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E292" s="27" t="s">
+      <c r="E292" s="26" t="s">
         <v>659</v>
       </c>
-      <c r="F292" s="23" t="s">
+      <c r="F292" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G292" s="23" t="s">
+      <c r="G292" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H292" s="23" t="s">
+      <c r="H292" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="293" ht="14.25">
+    <row r="293" ht="42.75">
       <c r="A293" s="5">
         <v>292</v>
       </c>
       <c r="B293" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C293" s="23" t="s">
+      <c r="C293" s="22" t="s">
         <v>660</v>
       </c>
       <c r="D293" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E293" s="27" t="s">
+      <c r="E293" s="26" t="s">
         <v>661</v>
       </c>
-      <c r="F293" s="23" t="s">
+      <c r="F293" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G293" s="23" t="s">
+      <c r="G293" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H293" s="23" t="s">
+      <c r="H293" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="294" ht="14.25">
+    <row r="294" ht="42.75">
       <c r="A294" s="5">
         <v>293</v>
       </c>
       <c r="B294" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C294" s="23" t="s">
+      <c r="C294" s="22" t="s">
         <v>662</v>
       </c>
       <c r="D294" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E294" s="27" t="s">
+      <c r="E294" s="26" t="s">
         <v>663</v>
       </c>
-      <c r="F294" s="23" t="s">
+      <c r="F294" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G294" s="23" t="s">
+      <c r="G294" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H294" s="23" t="s">
+      <c r="H294" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="295" ht="14.25">
+    <row r="295" ht="42.75">
       <c r="A295" s="5">
         <v>294</v>
       </c>
       <c r="B295" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C295" s="23" t="s">
+      <c r="C295" s="22" t="s">
         <v>664</v>
       </c>
       <c r="D295" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E295" s="27" t="s">
+      <c r="E295" s="26" t="s">
         <v>665</v>
       </c>
-      <c r="F295" s="23" t="s">
+      <c r="F295" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G295" s="23" t="s">
+      <c r="G295" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H295" s="23" t="s">
+      <c r="H295" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="296" ht="14.25">
+    <row r="296" ht="42.75">
       <c r="A296" s="5">
         <v>295</v>
       </c>
       <c r="B296" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C296" s="23" t="s">
+      <c r="C296" s="22" t="s">
         <v>666</v>
       </c>
       <c r="D296" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E296" s="27" t="s">
+      <c r="E296" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F296" s="23" t="s">
+      <c r="F296" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G296" s="23" t="s">
+      <c r="G296" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H296" s="23" t="s">
+      <c r="H296" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="297" ht="14.25">
+    <row r="297" ht="42.75">
       <c r="A297" s="5">
         <v>296</v>
       </c>
       <c r="B297" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C297" s="23" t="s">
+      <c r="C297" s="22" t="s">
         <v>667</v>
       </c>
       <c r="D297" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E297" s="27" t="s">
+      <c r="E297" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="F297" s="23" t="s">
+      <c r="F297" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G297" s="23" t="s">
+      <c r="G297" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H297" s="23" t="s">
+      <c r="H297" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="298" ht="14.25">
+    <row r="298" ht="42.75">
       <c r="A298" s="5">
         <v>297</v>
       </c>
       <c r="B298" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C298" s="23" t="s">
+      <c r="C298" s="22" t="s">
         <v>668</v>
       </c>
       <c r="D298" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E298" s="27" t="s">
+      <c r="E298" s="26" t="s">
         <v>669</v>
       </c>
-      <c r="F298" s="23" t="s">
+      <c r="F298" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G298" s="23" t="s">
+      <c r="G298" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H298" s="23" t="s">
+      <c r="H298" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="299" ht="14.25">
+    <row r="299" ht="42.75">
       <c r="A299" s="5">
         <v>298</v>
       </c>
       <c r="B299" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C299" s="23" t="s">
+      <c r="C299" s="22" t="s">
         <v>670</v>
       </c>
       <c r="D299" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E299" s="27" t="s">
+      <c r="E299" s="26" t="s">
         <v>671</v>
       </c>
-      <c r="F299" s="23" t="s">
+      <c r="F299" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G299" s="23" t="s">
+      <c r="G299" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H299" s="23" t="s">
+      <c r="H299" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="300" ht="14.25">
+    <row r="300" ht="42.75">
       <c r="A300" s="5">
         <v>299</v>
       </c>
       <c r="B300" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C300" s="23" t="s">
+      <c r="C300" s="22" t="s">
         <v>672</v>
       </c>
       <c r="D300" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E300" s="27" t="s">
+      <c r="E300" s="26" t="s">
         <v>673</v>
       </c>
-      <c r="F300" s="23" t="s">
+      <c r="F300" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G300" s="23" t="s">
+      <c r="G300" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H300" s="23" t="s">
+      <c r="H300" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="301" ht="14.25">
+    <row r="301" ht="42.75">
       <c r="A301" s="5">
         <v>300</v>
       </c>
       <c r="B301" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C301" s="23" t="s">
+      <c r="C301" s="22" t="s">
         <v>674</v>
       </c>
       <c r="D301" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E301" s="27" t="s">
+      <c r="E301" s="26" t="s">
         <v>675</v>
       </c>
-      <c r="F301" s="23" t="s">
+      <c r="F301" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G301" s="23" t="s">
+      <c r="G301" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H301" s="23" t="s">
+      <c r="H301" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="302" ht="14.25">
+    <row r="302" ht="42.75">
       <c r="A302" s="5">
         <v>301</v>
       </c>
       <c r="B302" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C302" s="23" t="s">
+      <c r="C302" s="22" t="s">
         <v>676</v>
       </c>
       <c r="D302" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E302" s="27" t="s">
+      <c r="E302" s="26" t="s">
         <v>677</v>
       </c>
-      <c r="F302" s="23" t="s">
+      <c r="F302" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G302" s="23" t="s">
+      <c r="G302" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H302" s="23" t="s">
+      <c r="H302" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="303" ht="14.25">
+    <row r="303" ht="42.75">
       <c r="A303" s="5">
         <v>302</v>
       </c>
       <c r="B303" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C303" s="23" t="s">
+      <c r="C303" s="22" t="s">
         <v>678</v>
       </c>
       <c r="D303" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E303" s="27" t="s">
+      <c r="E303" s="26" t="s">
         <v>679</v>
       </c>
-      <c r="F303" s="23" t="s">
+      <c r="F303" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G303" s="23" t="s">
+      <c r="G303" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H303" s="23" t="s">
+      <c r="H303" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="304" ht="14.25">
+    <row r="304" ht="42.75">
       <c r="A304" s="5">
         <v>303</v>
       </c>
       <c r="B304" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C304" s="23" t="s">
+      <c r="C304" s="22" t="s">
         <v>680</v>
       </c>
       <c r="D304" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E304" s="27" t="s">
+      <c r="E304" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F304" s="23" t="s">
+      <c r="F304" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G304" s="23" t="s">
+      <c r="G304" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H304" s="23" t="s">
+      <c r="H304" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="305" ht="14.25">
+    <row r="305" ht="42.75">
       <c r="A305" s="5">
         <v>304</v>
       </c>
       <c r="B305" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C305" s="23" t="s">
+      <c r="C305" s="22" t="s">
         <v>681</v>
       </c>
       <c r="D305" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E305" s="27" t="s">
+      <c r="E305" s="26" t="s">
         <v>682</v>
       </c>
-      <c r="F305" s="23" t="s">
+      <c r="F305" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G305" s="23" t="s">
+      <c r="G305" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H305" s="23" t="s">
+      <c r="H305" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="306" ht="14.25">
+    <row r="306" ht="42.75">
       <c r="A306" s="5">
         <v>305</v>
       </c>
       <c r="B306" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C306" s="23" t="s">
+      <c r="C306" s="22" t="s">
         <v>683</v>
       </c>
       <c r="D306" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E306" s="27" t="s">
+      <c r="E306" s="26" t="s">
         <v>684</v>
       </c>
-      <c r="F306" s="23" t="s">
+      <c r="F306" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G306" s="23" t="s">
+      <c r="G306" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H306" s="23" t="s">
+      <c r="H306" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="307" ht="14.25">
+    <row r="307" ht="42.75">
       <c r="A307" s="5">
         <v>306</v>
       </c>
       <c r="B307" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C307" s="23" t="s">
+      <c r="C307" s="22" t="s">
         <v>685</v>
       </c>
       <c r="D307" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E307" s="27" t="s">
+      <c r="E307" s="26" t="s">
         <v>686</v>
       </c>
-      <c r="F307" s="23" t="s">
+      <c r="F307" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="G307" s="23" t="s">
+      <c r="G307" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="H307" s="23" t="s">
+      <c r="H307" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="308" ht="14.25">
+    <row r="308" ht="42.75">
       <c r="A308" s="5">
         <v>307</v>
       </c>
@@ -10831,7 +10826,7 @@
       <c r="D308" s="18" t="s">
         <v>688</v>
       </c>
-      <c r="E308" s="19" t="s">
+      <c r="E308" s="12" t="s">
         <v>33</v>
       </c>
       <c r="F308" s="13" t="s">
@@ -10844,7 +10839,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="309" ht="14.25">
+    <row r="309" ht="42.75">
       <c r="A309" s="5">
         <v>308</v>
       </c>
@@ -10857,7 +10852,7 @@
       <c r="D309" s="18" t="s">
         <v>688</v>
       </c>
-      <c r="E309" s="19" t="s">
+      <c r="E309" s="12" t="s">
         <v>133</v>
       </c>
       <c r="F309" s="13" t="s">
@@ -10870,7 +10865,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="310" ht="14.25">
+    <row r="310" ht="42.75">
       <c r="A310" s="5">
         <v>309</v>
       </c>
@@ -10883,7 +10878,7 @@
       <c r="D310" s="18" t="s">
         <v>688</v>
       </c>
-      <c r="E310" s="19" t="s">
+      <c r="E310" s="12" t="s">
         <v>173</v>
       </c>
       <c r="F310" s="13" t="s">
@@ -10896,33 +10891,33 @@
         <v>106</v>
       </c>
     </row>
-    <row r="311" ht="14.25">
+    <row r="311" ht="42.75">
       <c r="A311" s="5">
         <v>310</v>
       </c>
       <c r="B311" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C311" s="23" t="s">
+      <c r="C311" s="22" t="s">
         <v>691</v>
       </c>
       <c r="D311" s="18" t="s">
         <v>688</v>
       </c>
-      <c r="E311" s="27" t="s">
+      <c r="E311" s="26" t="s">
         <v>570</v>
       </c>
-      <c r="F311" s="22" t="s">
+      <c r="F311" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="G311" s="23" t="s">
+      <c r="G311" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H311" s="23" t="s">
+      <c r="H311" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="312" ht="14.25">
+    <row r="312" ht="42.75">
       <c r="A312" s="5">
         <v>311</v>
       </c>
@@ -10935,7 +10930,7 @@
       <c r="D312" s="18" t="s">
         <v>688</v>
       </c>
-      <c r="E312" s="19" t="s">
+      <c r="E312" s="12" t="s">
         <v>77</v>
       </c>
       <c r="F312" s="13" t="s">
@@ -10948,7 +10943,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="313" ht="14.25">
+    <row r="313" ht="42.75">
       <c r="A313" s="5">
         <v>312</v>
       </c>
@@ -10961,7 +10956,7 @@
       <c r="D313" s="18" t="s">
         <v>688</v>
       </c>
-      <c r="E313" s="19" t="s">
+      <c r="E313" s="12" t="s">
         <v>75</v>
       </c>
       <c r="F313" s="13" t="s">
@@ -10974,7 +10969,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="314" ht="14.25">
+    <row r="314" ht="42.75">
       <c r="A314" s="5">
         <v>313</v>
       </c>
@@ -10987,7 +10982,7 @@
       <c r="D314" s="18" t="s">
         <v>688</v>
       </c>
-      <c r="E314" s="19" t="s">
+      <c r="E314" s="12" t="s">
         <v>42</v>
       </c>
       <c r="F314" s="13" t="s">
@@ -11000,7 +10995,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="315" ht="14.25">
+    <row r="315" ht="42.75">
       <c r="A315" s="5">
         <v>314</v>
       </c>
@@ -11013,7 +11008,7 @@
       <c r="D315" s="18" t="s">
         <v>688</v>
       </c>
-      <c r="E315" s="19" t="s">
+      <c r="E315" s="12" t="s">
         <v>165</v>
       </c>
       <c r="F315" s="13" t="s">
@@ -11026,7 +11021,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="316" ht="14.25">
+    <row r="316" ht="42.75">
       <c r="A316" s="5">
         <v>315</v>
       </c>
@@ -11039,7 +11034,7 @@
       <c r="D316" s="18" t="s">
         <v>688</v>
       </c>
-      <c r="E316" s="19" t="s">
+      <c r="E316" s="12" t="s">
         <v>94</v>
       </c>
       <c r="F316" s="13" t="s">
@@ -11052,7 +11047,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="317" ht="14.25">
+    <row r="317" ht="42.75">
       <c r="A317" s="5">
         <v>316</v>
       </c>
@@ -11065,7 +11060,7 @@
       <c r="D317" s="18" t="s">
         <v>688</v>
       </c>
-      <c r="E317" s="19" t="s">
+      <c r="E317" s="12" t="s">
         <v>141</v>
       </c>
       <c r="F317" s="13" t="s">
@@ -11079,7 +11074,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:H64"/>
+  <autoFilter ref="C1:H317"/>
   <sortState ref="C2:H4">
     <sortCondition ref="C2:C4"/>
   </sortState>
@@ -11091,7 +11086,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="5" id="{00B400CD-0012-4F33-A3F7-004B00DC009B}">
+          <x14:cfRule type="duplicateValues" priority="5" id="{002D0023-00C9-492F-AB88-001200DC001E}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -11107,7 +11102,7 @@
           <xm:sqref>E120:E166</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="8" id="{00B400D6-00F6-46AA-91BD-009900B100CD}">
+          <x14:cfRule type="duplicateValues" priority="8" id="{009E0066-0096-4844-A927-0001007F00E0}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -11123,7 +11118,7 @@
           <xm:sqref>E117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="3" id="{005300A6-00C2-43E9-95E5-007A00290094}">
+          <x14:cfRule type="duplicateValues" priority="3" id="{009E00B4-0032-45D0-9BB8-004600D900C4}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -11139,7 +11134,7 @@
           <xm:sqref>E118</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="1" id="{00E80011-003D-434D-B5C3-006900F6004B}">
+          <x14:cfRule type="duplicateValues" priority="1" id="{00160013-0046-47F7-B617-00B200E800AF}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -11155,7 +11150,7 @@
           <xm:sqref>E119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="6" id="{003C0001-008D-4E6F-9F2C-00C0005C0019}">
+          <x14:cfRule type="duplicateValues" priority="6" id="{00D0007F-0012-44EF-B909-00EE00260022}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>

</xml_diff>